<commit_message>
Update BOM Release V0
</commit_message>
<xml_diff>
--- a/H26R00/Released/BOM/H26R00.xlsx
+++ b/H26R00/Released/BOM/H26R00.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Hexabitz\Hardware\Eagle\Current\H26R00\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hexabitz_Github\Hardware\H26R0x-Hardware\H26R00\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1124D927-7317-4354-870D-47150A957FBA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEB6F27-4F38-4B09-B20B-EB7BA15C34F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="91">
   <si>
     <t>Qty</t>
   </si>
@@ -193,9 +193,6 @@
     <t>https://octopart.com/mmz1608y300b-tdk-368280?r=sp&amp;s=cd9_2ZEqQ9q9UNBuQgHAiA</t>
   </si>
   <si>
-    <t>P2</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
     <t>IC MCU 32BIT 128KB FLASH 48QFPN</t>
   </si>
   <si>
-    <t>P3</t>
-  </si>
-  <si>
     <t>CAP CER 1UF 16V X7R 0805</t>
   </si>
   <si>
@@ -250,18 +244,12 @@
     <t>C1</t>
   </si>
   <si>
-    <t>C3, C5, C6, C8, C9, C11, C12, C14, C15, C16</t>
-  </si>
-  <si>
     <t>C4, C7</t>
   </si>
   <si>
     <t>10uF</t>
   </si>
   <si>
-    <t>C10, C13</t>
-  </si>
-  <si>
     <t>CON-PHOENIX-350_1751277</t>
   </si>
   <si>
@@ -283,21 +271,6 @@
     <t>5pin Terminal Block; Printed Circuit; 10 A; 160 V; 3.5 mm; 5; 3.5 mm; 1.2 mm; M2; PA</t>
   </si>
   <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Diodes Incorporated</t>
-  </si>
-  <si>
-    <t>MMBT3906-7-F</t>
-  </si>
-  <si>
-    <t>https://octopart.com/mmbt3906-7-f-diodes+inc.-39667659?r=sp&amp;s=_q6BAroxTke1PVh8gNaaKg</t>
-  </si>
-  <si>
-    <t>PNP TRANSISTOR SOT23</t>
-  </si>
-  <si>
     <t>R4, R5, R6, R7</t>
   </si>
   <si>
@@ -316,16 +289,61 @@
     <t>24-Bit Analog-to-Digital Converter (ADC) for Weigh Scales</t>
   </si>
   <si>
-    <t>GRM188R60J106ME84D</t>
-  </si>
-  <si>
-    <t>https://octopart.com/grm188r60j106me84d-murata-29304413?r=sp&amp;s=F9Unx6EgTSWzmA_eGoaEng</t>
-  </si>
-  <si>
-    <t>CAP CER 10UF 6.3V X7R 0603</t>
-  </si>
-  <si>
-    <t>R3, R8, R9</t>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>LM2775-Q1</t>
+  </si>
+  <si>
+    <t>LM2775QDSGRQ1</t>
+  </si>
+  <si>
+    <t>https://octopart.com/lm2775qdsgrq1-texas+instruments-93339195?r=sp&amp;s=OA7oim0HQqaBsU4tLKFWXg LM2775QDSGRQ1</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>Switched Capacitor 5V Boost Converter 8-WSON -40 to 125</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>C3, C5, C6, C8, C9, C11, C12, C14, C15</t>
+  </si>
+  <si>
+    <t>C10, C13, C17</t>
+  </si>
+  <si>
+    <t>https://octopart.com/grm188r61a106ke69d-murata-22851381?r=ap&amp;s=o9t4ILLiSny6rfdd0oM5Kg</t>
+  </si>
+  <si>
+    <t>GRM188R61A106KE69D</t>
+  </si>
+  <si>
+    <t>https://octopart.com/grm188r61a105ka61j-murata-9221870?r=sp&amp;s=wvtiDxTpS1CkWsFaa2pliQ</t>
+  </si>
+  <si>
+    <t>GRM188R61A105KA61J</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 10V X5R 0603</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 10V X5R 0603</t>
+  </si>
+  <si>
+    <t>https://octopart.com/hx711-avia+semiconductor-106772965?r=sp&amp;s=oPimE1kgSpuO9TK8ujI3IA#</t>
   </si>
 </sst>
 </file>
@@ -397,7 +415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -417,6 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -760,33 +779,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.26171875" customWidth="1"/>
-    <col min="2" max="2" width="21.5234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.47265625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="60.47265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5234375" customWidth="1"/>
-    <col min="6" max="6" width="20.47265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.5234375" customWidth="1"/>
-    <col min="8" max="8" width="6.26171875" customWidth="1"/>
+    <col min="1" max="1" width="6.265625" customWidth="1"/>
+    <col min="2" max="2" width="21.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.46484375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="60.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.53125" customWidth="1"/>
+    <col min="6" max="6" width="20.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.53125" customWidth="1"/>
+    <col min="8" max="8" width="6.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -804,15 +823,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -827,7 +846,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -838,7 +857,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -850,191 +869,191 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1984646</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1984617</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1984646</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1984617</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="12" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1057,15 +1076,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
@@ -1080,7 +1099,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -1088,7 +1107,7 @@
         <v>100</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
@@ -1097,13 +1116,13 @@
         <v>10</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1114,7 +1133,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>7</v>
@@ -1126,58 +1145,85 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>74</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="G18" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{6E450E17-99C7-4DD0-97D5-E09D8479D56E}"/>
-    <hyperlink ref="G10" r:id="rId2" xr:uid="{FE09B789-44B6-4858-B584-84DE0ED1F18C}"/>
+    <hyperlink ref="G6" r:id="rId1" xr:uid="{6E450E17-99C7-4DD0-97D5-E09D8479D56E}"/>
+    <hyperlink ref="G11" r:id="rId2" xr:uid="{FE09B789-44B6-4858-B584-84DE0ED1F18C}"/>
     <hyperlink ref="G14" r:id="rId3" xr:uid="{0DEDC461-3D97-42B5-91BC-449136AA4DBD}"/>
+    <hyperlink ref="G16" r:id="rId4" xr:uid="{124CA29A-E8B7-47DF-AA23-DCD384315728}"/>
+    <hyperlink ref="G17" r:id="rId5" display="https://octopart.com/hx711-avia+semiconductor-106772965?r=sp&amp;s=oPimE1kgSpuO9TK8ujI3IA" xr:uid="{D43B0DED-D379-4AD2-A8E7-F44B83EA1C2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1187,7 +1233,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1199,7 +1245,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>